<commit_message>
copy ids from column 9 to 1 and sort and deleted dubicate
</commit_message>
<xml_diff>
--- a/Work/HM_updated.xlsx
+++ b/Work/HM_updated.xlsx
@@ -526,6 +526,11 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0713995026</t>
+        </is>
+      </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1041592001.html</t>
@@ -579,6 +584,11 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0714790050</t>
+        </is>
+      </c>
       <c r="H3" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1041592001.html</t>
@@ -632,6 +642,11 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0834677001</t>
+        </is>
+      </c>
       <c r="H4" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1041592001.html</t>
@@ -685,6 +700,11 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0838901008</t>
+        </is>
+      </c>
       <c r="H5" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1041592001.html</t>
@@ -738,6 +758,11 @@
       </c>
     </row>
     <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>0867725004</t>
+        </is>
+      </c>
       <c r="H6" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.0713995026.html</t>
@@ -791,6 +816,11 @@
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>0915573001</t>
+        </is>
+      </c>
       <c r="H7" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.0713995026.html</t>
@@ -844,6 +874,11 @@
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>0916881006</t>
+        </is>
+      </c>
       <c r="H8" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.0713995026.html</t>
@@ -897,6 +932,11 @@
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>0934389001</t>
+        </is>
+      </c>
       <c r="H9" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.0995747001.html</t>
@@ -914,6 +954,11 @@
       <c r="R9" s="1" t="inlineStr"/>
     </row>
     <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>0934389004</t>
+        </is>
+      </c>
       <c r="H10" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1009117001.html</t>
@@ -931,6 +976,11 @@
       <c r="R10" s="1" t="inlineStr"/>
     </row>
     <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>0937627006</t>
+        </is>
+      </c>
       <c r="H11" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1023104001.html</t>
@@ -976,6 +1026,11 @@
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>0966548006</t>
+        </is>
+      </c>
       <c r="H12" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1023104001.html</t>
@@ -1021,6 +1076,11 @@
       </c>
     </row>
     <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>0980639002</t>
+        </is>
+      </c>
       <c r="H13" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1012755001.html</t>
@@ -1066,6 +1126,11 @@
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>0990958002</t>
+        </is>
+      </c>
       <c r="H14" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1012755001.html</t>
@@ -1111,6 +1176,11 @@
       </c>
     </row>
     <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>0994093003</t>
+        </is>
+      </c>
       <c r="H15" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.0925376025.html</t>
@@ -1128,6 +1198,11 @@
       <c r="R15" s="1" t="inlineStr"/>
     </row>
     <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1003246001</t>
+        </is>
+      </c>
       <c r="H16" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1023660004.html</t>
@@ -1145,6 +1220,11 @@
       <c r="R16" s="1" t="inlineStr"/>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1006274002</t>
+        </is>
+      </c>
       <c r="H17" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.0990958002.html</t>
@@ -1194,6 +1274,11 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1006374001</t>
+        </is>
+      </c>
       <c r="H18" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.0990958002.html</t>
@@ -1243,6 +1328,11 @@
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1009052002</t>
+        </is>
+      </c>
       <c r="H19" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.0714790050.html</t>
@@ -1292,6 +1382,11 @@
       </c>
     </row>
     <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>1011255001</t>
+        </is>
+      </c>
       <c r="H20" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.0714790050.html</t>
@@ -1341,6 +1436,11 @@
       </c>
     </row>
     <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>1012755001</t>
+        </is>
+      </c>
       <c r="H21" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1061581001.html</t>
@@ -1394,6 +1494,11 @@
       </c>
     </row>
     <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>1019603001</t>
+        </is>
+      </c>
       <c r="H22" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1061581001.html</t>
@@ -1447,6 +1552,11 @@
       </c>
     </row>
     <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>1023104001</t>
+        </is>
+      </c>
       <c r="H23" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.0994093003.html</t>
@@ -1492,6 +1602,11 @@
       </c>
     </row>
     <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>1024871002</t>
+        </is>
+      </c>
       <c r="H24" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.0994093003.html</t>
@@ -1537,6 +1652,11 @@
       </c>
     </row>
     <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>1027978002</t>
+        </is>
+      </c>
       <c r="H25" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1041278003.html</t>
@@ -1582,6 +1702,11 @@
       </c>
     </row>
     <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>1032158001</t>
+        </is>
+      </c>
       <c r="H26" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1041278003.html</t>
@@ -1627,6 +1752,11 @@
       </c>
     </row>
     <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>1037082006</t>
+        </is>
+      </c>
       <c r="H27" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1032158001.html</t>
@@ -1672,6 +1802,11 @@
       </c>
     </row>
     <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>1041278003</t>
+        </is>
+      </c>
       <c r="H28" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1032158001.html</t>
@@ -1717,6 +1852,11 @@
       </c>
     </row>
     <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>1041556002</t>
+        </is>
+      </c>
       <c r="H29" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1037082006.html</t>
@@ -1766,6 +1906,11 @@
       </c>
     </row>
     <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>1041592001</t>
+        </is>
+      </c>
       <c r="H30" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1037082006.html</t>
@@ -1815,6 +1960,11 @@
       </c>
     </row>
     <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>1052145001</t>
+        </is>
+      </c>
       <c r="H31" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1037082006.html</t>
@@ -1864,6 +2014,11 @@
       </c>
     </row>
     <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>1061581001</t>
+        </is>
+      </c>
       <c r="H32" s="1" t="inlineStr">
         <is>
           <t>https://www2.hm.com/pl_pl/productpage.1037082006.html</t>

</xml_diff>